<commit_message>
se agrega archivo pbix Spring 4 y parcialdocumentación en md
</commit_message>
<xml_diff>
--- a/SPRING_4/reports_dframes/comparativa_ventas_23_24_pBI.xlsx
+++ b/SPRING_4/reports_dframes/comparativa_ventas_23_24_pBI.xlsx
@@ -7,9 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Resumen" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Top_Productos_2023" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Top_Productos_2024" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Resumen_Años" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Productos_2023" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Productos_2024" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -448,23 +448,19 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
+      <c r="A2" t="n">
+        <v>2023</v>
       </c>
       <c r="B2" t="n">
-        <v>100051.253375</v>
+        <v>100051.25</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2024</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2024</v>
       </c>
       <c r="B3" t="n">
-        <v>65388.921175</v>
+        <v>65388.92</v>
       </c>
     </row>
   </sheetData>
@@ -478,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A133"/>
+  <dimension ref="A1:B133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,667 +485,1332 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>monto_final</t>
+          <t>nombre_producto_x</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ventas_producto</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2075.2</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Sprite 1.5L</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2075.2002</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1922.23</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Yerba Mate Suave 1kg</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1922.22765</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>1855.8</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pepsi 1.5L</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1855.799275</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1792.35</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Empanadas Congeladas</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1792.34725</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1751.9</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Pizza Congelada Muzzarella</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1751.9025</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1712.44</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Desodorante Ambiente Aerosol</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1712.43625</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>1696.43</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Agua Mineral 500ml</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1696.432125</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>1679.47</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Queso Rallado 150g</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1679.4666</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>1660.65</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Detergente Ropa Color 800g</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1660.647975</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>1659.12</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ron 700ml</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1659.1218</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>1643.61</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Queso Azul 150g</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1643.6105</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>1628.82</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Queso Cremoso 500g</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1628.8163</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>1595.61</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Miel Pura 250g</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1595.61005</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>1583.75</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Jugo en Polvo Limón</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1583.75025</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>1375.35</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Esponja de Limpieza</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1375.3476</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>1364.9</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Fernet 750ml</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1364.9021</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>1361.06</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Detergente Lavavajillas 500ml</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1361.0634</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>1349.52</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Aceitunas Verdes 200g</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1349.523</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>1332.63</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Jugo de Naranja 1L</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1332.62775</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>1326.36</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Granola 250g</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1326.363025</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>1303.6</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Mix de Frutos Secos 200g</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1303.6016</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>1291.25</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Harina Leudante 1kg</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1291.248</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>1246.26</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Yerba Mate Intensa 1kg</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1246.263675</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>1240.15</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Mostaza 250g</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1240.1505</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>1233.67</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Tostadas Integrales</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1233.66775</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Chicle Menta</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
         <v>1228.08</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>1161.12</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Whisky 750ml</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1161.1196</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Mayonesa 250g</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
         <v>1156.85</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>1150.85</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Fideos Secos Tallarines 500g</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1150.8464</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>1102.83</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Bizcochos Salados</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1102.8325</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>1101.4</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Hamburguesas Congeladas x4</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1101.4025</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Repelente de Insectos</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
         <v>1060.99</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>1044.02</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Aceitunas Negras 200g</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1044.0234</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>1035.21</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Stevia 100 sobres</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1035.2082</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>1010.36</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Yogur Natural 200g</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1010.362325</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>948.38</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Desinfectante Aerosol</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>948.38465</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>945.3</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Vino Blanco 750ml</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>945.3048</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Desodorante Aerosol</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
         <v>938</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>921.5</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Palitos Salados</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>921.496875</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>919.73</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Energética Nitro 500ml</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>919.7349</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>899.12</v>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Ketchup 250g</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>899.1246500000001</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>895.21</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Mermelada de Frutilla 400g</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>895.2120000000001</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>885.25</v>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Chupetín</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>885.2535</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>882.21</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Avena Instantánea 250g</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>882.210775</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>880.91</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Jugo de Manzana 1L</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>880.9137749999999</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>880.39</v>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Maní Salado 200g</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>880.3896999999999</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>859.72</v>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Fideos Secos Tirabuzones 500g</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>859.7193</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>853.0599999999999</v>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Aceite de Girasol 900ml</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>853.0624</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>850.04</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Lavandina 1L</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>850.04195</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>833.53</v>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Toallas Húmedas x50</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>833.5269499999999</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>830.27</v>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Suavizante Ropa 900ml</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>830.2658000000001</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>829.53</v>
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Aceite de Oliva 500ml</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>829.52815</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>823.67</v>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Licor de Café 700ml</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>823.6683</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>790.25</v>
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Arroz Largo Fino 1kg</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>790.254225</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="n">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Harina de Trigo 1kg</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
         <v>789.51</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="n">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Verduras Congeladas Mix</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
         <v>772.02</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>759.71</v>
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Premezcla para Pizza</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>759.713</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>753.09</v>
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Queso Untable 190g</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>753.0907500000001</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>747.37</v>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Medialunas de Manteca</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>747.3745250000001</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>742.71</v>
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Helado Chocolate 1L</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>742.7084</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
-        <v>742.52</v>
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Sal Fina 500g</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>742.51575</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>741.35</v>
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Cepillo de Dientes</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>741.3462000000001</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="n">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Cerveza Negra 1L</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
         <v>720.51</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="n">
-        <v>719.34</v>
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Azúcar 1kg</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>719.34345</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>707.61</v>
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Jabón de Tocador x3</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>707.6079999999999</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>694.48</v>
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Bloqueador Solar SPF 50</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>694.485</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>693.35</v>
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Helado de Frutilla 1L</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>693.3499999999999</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>692.1</v>
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Garbanzos 500g</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>692.09685</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>687.26</v>
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Fanta Naranja 1.5L</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>687.2556499999999</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="n">
-        <v>677.14</v>
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Leche Descremada 1L</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>677.1383999999999</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="n">
-        <v>665.28</v>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Caramelos Masticables</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>665.2800000000001</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="n">
-        <v>638.76</v>
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Té Verde 20 saquitos</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>638.76315</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="n">
-        <v>617.34</v>
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Dulce de Leche 400g</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>617.3433</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="n">
-        <v>617.27</v>
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Jabón en Polvo 800g</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>617.273775</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="n">
-        <v>608.42</v>
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Cerveza Rubia 1L</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>608.4153</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="n">
-        <v>608.1799999999999</v>
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Aceite de Girasol 1L</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>608.1808249999999</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="n">
-        <v>585.9</v>
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Premezcla para Pan</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>585.9000000000001</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="n">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Coca Cola 1.5L</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
         <v>563.28</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="n">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Limpiador de Pisos 1L</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
         <v>558.87</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="n">
-        <v>549.75</v>
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Galletitas Saladas</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>549.75275</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="n">
-        <v>547.88</v>
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Vino Tinto Malbec 750ml</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>547.8759</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="n">
-        <v>541.45</v>
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Leche Entera 1L</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>541.45275</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="n">
-        <v>541.16</v>
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Chocolate Amargo 100g</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>541.1553</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="n">
-        <v>534.1900000000001</v>
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Trapo de Piso</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>534.1949500000001</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="n">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Snack de Queso</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
         <v>522</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="n">
-        <v>514.3200000000001</v>
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Crema Dental 90g</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>514.3199999999999</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="n">
-        <v>512.16</v>
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Gin 700ml</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>512.1641</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="n">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Obleas de Chocolate</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
         <v>485.76</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="n">
-        <v>482.08</v>
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Pasta Dental 90g</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>482.0836</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="n">
-        <v>481.31</v>
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Jugo en Polvo Naranja</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>481.3072</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="n">
-        <v>479.73</v>
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Barritas de Cereal</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>479.7287</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="n">
-        <v>476.91</v>
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Café Molido 250g</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>476.9119</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="n">
-        <v>473.97</v>
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Galletitas Vainilla</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>473.97075</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="n">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Manteca 200g</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
         <v>455.14</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="n">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Acondicionador 400ml</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
         <v>445.9</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="n">
-        <v>440.6</v>
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Desengrasante 500ml</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>440.5995</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="n">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Jabón de Tocador</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
         <v>419.7</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="n">
-        <v>413.58</v>
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Gelatina Sabor Frutilla</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>413.5752</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="n">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Limpiavidrios 500ml</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
         <v>409.84</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="n">
-        <v>374.47</v>
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Shampoo 400ml</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>374.47305</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="n">
-        <v>364.32</v>
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Fideos Spaghetti 500g</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>364.3199999999999</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="n">
-        <v>359.59</v>
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Salsa de Tomate 500g</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>359.5898</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="n">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Caldo Concentrado Carne</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
         <v>356.72</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="n">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Servilletas x100</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
         <v>343.92</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="n">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Pan Lactal Blanco</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
         <v>343.16</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="n">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Sopa Instantánea Pollo</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
         <v>335.76</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="n">
-        <v>320.41</v>
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Mascarilla Capilar</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>320.408</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="n">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Hilo Dental</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
         <v>300.23</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="n">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Barrita de Cereal 30g</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
         <v>293.48</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="n">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Galletitas Chocolate</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
         <v>276.1</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="n">
-        <v>257.91</v>
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Papas Fritas Bolsa Grande</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>257.9073</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="n">
-        <v>242.67</v>
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Papas Fritas Onduladas 100g</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>242.6655</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="n">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Papel Higiénico x4</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
         <v>222.95</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="n">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Alcohol en Gel 500ml</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
         <v>217.91</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="n">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Papas Fritas Clásicas 100g</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
         <v>216</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="n">
-        <v>195.17</v>
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Té Negro 20 saquitos</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>195.168</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="n">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Mermelada de Durazno 400g</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
         <v>175.77</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="n">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Caldo Concentrado Verdura</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
         <v>171.96</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="n">
-        <v>157.17</v>
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Helado Vainilla 1L</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>157.173625</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="n">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Lentejas Secas 500g</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
         <v>151.8</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="n">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Lentejas 500g</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
         <v>146.16</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="n">
-        <v>145.62</v>
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Sidra 750ml</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>145.6194</v>
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="n">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Alfajor Simple</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
         <v>135.38</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="n">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Vinagre de Alcohol 500ml</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
         <v>120.56</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="n">
-        <v>93.12</v>
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Flan Casero en Polvo</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>93.117875</v>
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="n">
-        <v>92.06999999999999</v>
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Porotos Negros 500g</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>92.07000000000001</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="n">
-        <v>87.72</v>
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Detergente Líquido 750ml</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>87.723</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" t="n">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Vodka 700ml</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
         <v>76.2</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="n">
-        <v>70.67</v>
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Pan Lactal Integral</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>70.67240000000001</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="n">
-        <v>70.55</v>
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Turrón 50g</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>70.54575000000001</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="n">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Alfajor Triple</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
         <v>60.72</v>
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="n">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Chocolate con Leche 100g</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
         <v>44.28</v>
       </c>
     </row>
@@ -1164,7 +1825,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A101"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1175,508 +1836,1013 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>monto_final</t>
+          <t>nombre_producto_x</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ventas_producto</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>2131.91</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Sprite 1.5L</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2131.9139</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Yogur Natural 200g</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>1383.9</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>1362.98</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Mayonesa 250g</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1362.975</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Stevia 100 sobres</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>1341.99</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1317.04</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Pasta Dental 90g</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1317.044675</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Desodorante Ambiente Aerosol</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>1313.2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>1232.96</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Empanadas Congeladas</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1232.9629</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>1229.47</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Jugo de Manzana 1L</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1229.4709</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Palitos Salados</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>1170</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>1160.44</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Galletitas Vainilla</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1160.435375</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>1144.82</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Yerba Mate Intensa 1kg</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1144.81935</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>1120.39</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Verduras Congeladas Mix</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1120.394025</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>1106</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Pizza Congelada Muzzarella</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1106.0023</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>1097.92</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Fideos Secos Tallarines 500g</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1097.9188</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>1093.24</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Limpiador de Pisos 1L</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1093.2357</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>1076.29</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Suavizante Ropa 900ml</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1076.291125</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>1015.42</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Detergente Lavavajillas 500ml</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1015.4238</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>1011.12</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Mostaza 250g</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1011.123</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>1001.06</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Aceite de Girasol 900ml</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1001.064175</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>997.92</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Esponja de Limpieza</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>997.9200000000001</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>989.05</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Granola 250g</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>989.0528499999999</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>943.72</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Queso Cremoso 500g</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>943.71765</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>923.51</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Gelatina Sabor Frutilla</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>923.51475</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Ron 700ml</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
         <v>891.48</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>888.46</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Coca Cola 1.5L</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>888.4568499999999</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>886.34</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Mix de Frutos Secos 200g</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>886.3400000000001</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>847.89</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Premezcla para Pan</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>847.8949500000001</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>835.71</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Pepsi 1.5L</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>835.7126499999999</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>828.61</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Repelente de Insectos</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>828.610125</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>818.92</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Energética Nitro 500ml</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>818.9247</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>818.8099999999999</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Garbanzos 500g</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>818.8092</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>809.97</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Chupetín</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>809.9721</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>792.73</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Queso Azul 150g</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>792.7272499999999</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>791.52</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Jabón de Tocador x3</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>791.5214999999999</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>784.86</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Agua Mineral 500ml</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>784.8611000000001</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>776.97</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Detergente Ropa Color 800g</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>776.969625</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>761.8</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Aceitunas Verdes 200g</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>761.7959999999999</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>760.75</v>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Harina Leudante 1kg</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>760.7520000000001</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>721.42</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Whisky 750ml</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>721.4179</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>720.26</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Desinfectante Aerosol</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>720.2623</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Acondicionador 400ml</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
         <v>713.4400000000001</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>704.71</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Jugo en Polvo Limón</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>704.707</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Bloqueador Solar SPF 50</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
         <v>698.28</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>689.5700000000001</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Jabón en Polvo 800g</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>689.5671</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>682.91</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Miel Pura 250g</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>682.90765</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>680.95</v>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Vino Tinto Malbec 750ml</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>680.9517</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>672.09</v>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Obleas de Chocolate</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>672.0944999999999</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Premezcla para Pizza</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
         <v>667</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>655.47</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Azúcar 1kg</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>655.4737499999999</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>654.72</v>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Aceite de Oliva 500ml</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>654.71615</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>645.29</v>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Hamburguesas Congeladas x4</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>645.293</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>628.48</v>
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Tostadas Integrales</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>628.4793000000001</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>617.65</v>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Café Molido 250g</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>617.64505</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>614.05</v>
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Lentejas 500g</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>614.0547</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>609.58</v>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Helado Chocolate 1L</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>609.5824</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="n">
-        <v>582.46</v>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Alcohol en Gel 500ml</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>582.463525</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Arroz Largo Fino 1kg</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
         <v>566.01</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="n">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Galletitas Saladas</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
         <v>527.1</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>526.34</v>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Ketchup 250g</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>526.34465</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>523.29</v>
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Cepillo de Dientes</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>523.2906</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Harina de Trigo 1kg</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
         <v>507.78</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>501.46</v>
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Pan Lactal Blanco</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>501.4612</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="n">
-        <v>488.06</v>
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Queso Untable 190g</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>488.061</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="n">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Queso Rallado 150g</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
         <v>482.16</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>475.96</v>
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Barritas de Cereal</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>475.9574</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>474.97</v>
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Manteca 200g</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>474.9711</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>460.34</v>
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Té Verde 20 saquitos</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>460.3360249999999</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>450.92</v>
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Cerveza Rubia 1L</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>450.9203</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>431.33</v>
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Jugo en Polvo Naranja</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>431.3344</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="n">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Maní Salado 200g</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
         <v>430.22</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="n">
-        <v>418.77</v>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Medialunas de Manteca</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>418.7656</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="n">
-        <v>404.48</v>
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Yerba Mate Suave 1kg</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>404.4754</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="n">
-        <v>395.21</v>
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Gin 700ml</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>395.206175</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="n">
-        <v>363.7</v>
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Fanta Naranja 1.5L</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>363.7037</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="n">
-        <v>360.98</v>
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Fideos Secos Tirabuzones 500g</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>360.9804</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="n">
-        <v>338.73</v>
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Papas Fritas Bolsa Grande</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>338.72895</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="n">
-        <v>329.53</v>
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Jugo de Naranja 1L</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>329.53425</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="n">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Aceitunas Negras 200g</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
         <v>311.22</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="n">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Leche Entera 1L</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
         <v>310.14</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="n">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Snack de Queso</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
         <v>306</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="n">
-        <v>298.43</v>
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Sal Fina 500g</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>298.43275</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="n">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Chicle Menta</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
         <v>288.96</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="n">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Licor de Café 700ml</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
         <v>288.36</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="n">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Toallas Húmedas x50</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
         <v>261.18</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="n">
-        <v>246.24</v>
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Helado de Frutilla 1L</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>246.2383</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="n">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Shampoo 400ml</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
         <v>211.05</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="n">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Leche Descremada 1L</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
         <v>203.04</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="n">
-        <v>202.68</v>
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Salsa de Tomate 500g</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>202.6795</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="n">
-        <v>185.26</v>
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Vino Blanco 750ml</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>185.2631</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="n">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Vodka 700ml</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
         <v>172.72</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="n">
-        <v>169.24</v>
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Fernet 750ml</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>169.242175</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="n">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Bizcochos Salados</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
         <v>166.6</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="n">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Avena Instantánea 250g</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
         <v>158.12</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="n">
-        <v>154.13</v>
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Té Negro 20 saquitos</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>154.128</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="n">
-        <v>139.48</v>
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Sidra 750ml</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>139.4814</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="n">
-        <v>111.67</v>
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Helado Vainilla 1L</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>111.6689</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="n">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Cerveza Negra 1L</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
         <v>107.31</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="n">
-        <v>94.59</v>
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Flan Casero en Polvo</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>94.58915</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="n">
-        <v>73.38</v>
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Limpiavidrios 500ml</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>73.37880000000001</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="n">
-        <v>54.24</v>
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Pan Lactal Integral</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>54.2436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>